<commit_message>
That is some change!!!
</commit_message>
<xml_diff>
--- a/Student.xlsx
+++ b/Student.xlsx
@@ -377,7 +377,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -403,65 +403,65 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2">
-        <v>1</v>
+      <c r="A2" t="str">
+        <v>5e57ee1bcf822f37ca4dd4ab</v>
       </c>
       <c r="B2" t="str">
+        <v>Diyor</v>
+      </c>
+      <c r="C2" t="str">
+        <v>Dilmurod</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="F2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>5e57ee1bcf822f37ca4dd4ae</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Dell</v>
+      </c>
+      <c r="C3" t="str">
+        <v>Dilshod</v>
+      </c>
+      <c r="D3">
+        <v>6</v>
+      </c>
+      <c r="F3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>5e57ee1bcf822f37ca4dd4ad</v>
+      </c>
+      <c r="B4" t="str">
         <v>Dimok</v>
       </c>
-      <c r="C2" t="str">
-        <v>Saodat</v>
-      </c>
-      <c r="D2">
-        <v>7</v>
-      </c>
-      <c r="F2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3">
-        <v>5</v>
-      </c>
-      <c r="B3" t="str">
-        <v>Diyor</v>
-      </c>
-      <c r="C3" t="str">
-        <v>Dilmurod</v>
-      </c>
-      <c r="D3">
-        <v>5</v>
-      </c>
-      <c r="F3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4">
-        <v>4</v>
-      </c>
-      <c r="B4" t="str">
-        <v>Nodir</v>
-      </c>
       <c r="C4" t="str">
-        <v>Dilshod</v>
+        <v>Oyatillo</v>
       </c>
       <c r="D4">
         <v>5</v>
       </c>
       <c r="F4">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5">
-        <v>2</v>
+      <c r="A5" t="str">
+        <v>5e57ee1bcf822f37ca4dd4af</v>
       </c>
       <c r="B5" t="str">
-        <v>Aziza</v>
+        <v>Nodir</v>
       </c>
       <c r="C5" t="str">
-        <v>Dilmurod</v>
+        <v>Saodat</v>
       </c>
       <c r="D5">
         <v>5</v>
@@ -471,283 +471,283 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6">
-        <v>7</v>
+      <c r="A6" t="str">
+        <v>5e57ee1bcf822f37ca4dd4b0</v>
       </c>
       <c r="B6" t="str">
         <v>Dimok</v>
       </c>
       <c r="C6" t="str">
+        <v>Saodat</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="F6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>5e57ee1bcf822f37ca4dd4b1</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Diyor</v>
+      </c>
+      <c r="C7" t="str">
+        <v>Dilmurod</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>5e57ee1bcf822f37ca4dd4b2</v>
+      </c>
+      <c r="B8" t="str">
+        <v>Nodir</v>
+      </c>
+      <c r="C8" t="str">
         <v>Oyatillo</v>
       </c>
-      <c r="D6">
-        <v>5</v>
-      </c>
-      <c r="F6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7">
+      <c r="D8">
+        <v>6</v>
+      </c>
+      <c r="F8">
         <v>3</v>
       </c>
-      <c r="B7" t="str">
-        <v>Aziza</v>
-      </c>
-      <c r="C7" t="str">
-        <v>Oyatillo</v>
-      </c>
-      <c r="D7">
-        <v>6</v>
-      </c>
-      <c r="F7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8">
-        <v>8</v>
-      </c>
-      <c r="B8" t="str">
-        <v>Dell</v>
-      </c>
-      <c r="C8" t="str">
-        <v>Dilshod</v>
-      </c>
-      <c r="D8">
-        <v>6</v>
-      </c>
-      <c r="F8">
-        <v>4</v>
-      </c>
     </row>
     <row r="9">
-      <c r="A9">
-        <v>9</v>
+      <c r="A9" t="str">
+        <v>5e57ee1bcf822f37ca4dd4b3</v>
       </c>
       <c r="B9" t="str">
-        <v>Nodir</v>
+        <v>Dimok</v>
       </c>
       <c r="C9" t="str">
         <v>Saodat</v>
       </c>
       <c r="D9">
+        <v>7</v>
+      </c>
+      <c r="F9">
         <v>5</v>
       </c>
-      <c r="F9">
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>5e57ee1bcf822f37ca4dd4b4</v>
+      </c>
+      <c r="B10" t="str">
+        <v>Dell</v>
+      </c>
+      <c r="C10" t="str">
+        <v>Dilmurod</v>
+      </c>
+      <c r="D10">
+        <v>4</v>
+      </c>
+      <c r="F10">
         <v>2</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10">
-        <v>10</v>
-      </c>
-      <c r="B10" t="str">
-        <v>Dimok</v>
-      </c>
-      <c r="C10" t="str">
+    <row r="11">
+      <c r="A11" t="str">
+        <v>5e57ee1bcf822f37ca4dd4b5</v>
+      </c>
+      <c r="B11" t="str">
+        <v>Aziza</v>
+      </c>
+      <c r="C11" t="str">
         <v>Saodat</v>
       </c>
-      <c r="D10">
-        <v>4</v>
-      </c>
-      <c r="F10">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11">
-        <v>11</v>
-      </c>
-      <c r="B11" t="str">
-        <v>Diyor</v>
-      </c>
-      <c r="C11" t="str">
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="F11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>5e57ee1bcf822f37ca4dd4b6</v>
+      </c>
+      <c r="B12" t="str">
+        <v>Mamur</v>
+      </c>
+      <c r="C12" t="str">
+        <v>Navroz</v>
+      </c>
+      <c r="D12">
+        <v>4</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>5e57ee1bcf822f37ca4dd4b7</v>
+      </c>
+      <c r="B13" t="str">
+        <v>Nodir</v>
+      </c>
+      <c r="C13" t="str">
+        <v>Oyatillo</v>
+      </c>
+      <c r="D13">
+        <v>4</v>
+      </c>
+      <c r="F13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>5e57ee1bcf822f37ca4dd4b8</v>
+      </c>
+      <c r="B14" t="str">
+        <v>Aziza</v>
+      </c>
+      <c r="C14" t="str">
         <v>Dilmurod</v>
       </c>
-      <c r="D11">
-        <v>5</v>
-      </c>
-      <c r="F11">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12">
-        <v>12</v>
-      </c>
-      <c r="B12" t="str">
-        <v>Nodir</v>
-      </c>
-      <c r="C12" t="str">
-        <v>Oyatillo</v>
-      </c>
-      <c r="D12">
-        <v>6</v>
-      </c>
-      <c r="F12">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13">
-        <v>13</v>
-      </c>
-      <c r="B13" t="str">
-        <v>Dimok</v>
-      </c>
-      <c r="C13" t="str">
-        <v>Saodat</v>
-      </c>
-      <c r="D13">
+      <c r="D14">
         <v>7</v>
       </c>
-      <c r="F13">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14">
-        <v>6</v>
-      </c>
-      <c r="B14" t="str">
-        <v>Mamur</v>
-      </c>
-      <c r="C14" t="str">
-        <v>Saodat</v>
-      </c>
-      <c r="D14">
-        <v>4</v>
-      </c>
       <c r="F14">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15">
-        <v>14</v>
+      <c r="A15" t="str">
+        <v>5e57ee1bcf822f37ca4dd4b9</v>
       </c>
       <c r="B15" t="str">
-        <v>Dell</v>
+        <v>Sardor</v>
       </c>
       <c r="C15" t="str">
-        <v>Dilmurod</v>
+        <v>Dilshod</v>
       </c>
       <c r="D15">
         <v>4</v>
       </c>
       <c r="F15">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16">
-        <v>15</v>
+      <c r="A16" t="str">
+        <v>5e57ee1bcf822f37ca4dd4bc</v>
       </c>
       <c r="B16" t="str">
-        <v>Aziza</v>
+        <v>Nozi</v>
       </c>
       <c r="C16" t="str">
         <v>Saodat</v>
       </c>
       <c r="D16">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F16">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17">
-        <v>16</v>
+      <c r="A17" t="str">
+        <v>5e57ee1bcf822f37ca4dd4ba</v>
       </c>
       <c r="B17" t="str">
-        <v>Mamur</v>
+        <v>Dimok</v>
       </c>
       <c r="C17" t="str">
-        <v>Navroz</v>
+        <v>Dilmurod</v>
       </c>
       <c r="D17">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F17">
         <v>2</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18">
-        <v>17</v>
+      <c r="A18" t="str">
+        <v>5e57ee1bcf822f37ca4dd4bb</v>
       </c>
       <c r="B18" t="str">
-        <v>Nodir</v>
+        <v>Sardor</v>
       </c>
       <c r="C18" t="str">
-        <v>Oyatillo</v>
+        <v>Dilshod</v>
       </c>
       <c r="D18">
         <v>4</v>
       </c>
       <c r="F18">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19">
-        <v>18</v>
+      <c r="A19" t="str">
+        <v>5e57ee1bcf822f37ca4dd4bd</v>
       </c>
       <c r="B19" t="str">
         <v>Aziza</v>
       </c>
       <c r="C19" t="str">
-        <v>Dilmurod</v>
+        <v>Dilshod</v>
       </c>
       <c r="D19">
         <v>7</v>
       </c>
       <c r="F19">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20">
-        <v>19</v>
+      <c r="A20" t="str">
+        <v>5e57ee1bcf822f37ca4dd4be</v>
       </c>
       <c r="B20" t="str">
-        <v>Sardor</v>
+        <v>Mamur</v>
       </c>
       <c r="C20" t="str">
         <v>Dilshod</v>
       </c>
       <c r="D20">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F20">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21">
-        <v>20</v>
+      <c r="A21" t="str">
+        <v>5e57ee1bcf822f37ca4dd4bf</v>
       </c>
       <c r="B21" t="str">
-        <v>Dimok</v>
+        <v>Sardor</v>
       </c>
       <c r="C21" t="str">
-        <v>Dilmurod</v>
+        <v>Oyatillo</v>
       </c>
       <c r="D21">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F21">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22">
-        <v>21</v>
+      <c r="A22" t="str">
+        <v>5e57ee1bcf822f37ca4dd4c0</v>
       </c>
       <c r="B22" t="str">
-        <v>Sardor</v>
+        <v>Aziza</v>
       </c>
       <c r="C22" t="str">
         <v>Dilshod</v>
@@ -756,148 +756,63 @@
         <v>4</v>
       </c>
       <c r="F22">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23">
-        <v>22</v>
+      <c r="A23" t="str">
+        <v>5e57ee1bcf822f37ca4dd4c1</v>
       </c>
       <c r="B23" t="str">
-        <v>Nozi</v>
+        <v>Diyor</v>
       </c>
       <c r="C23" t="str">
-        <v>Saodat</v>
+        <v>Dilshod</v>
       </c>
       <c r="D23">
         <v>7</v>
       </c>
       <c r="F23">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24">
-        <v>23</v>
+      <c r="A24" t="str">
+        <v>5e57ee1bcf822f37ca4dd4c2</v>
       </c>
       <c r="B24" t="str">
-        <v>Aziza</v>
+        <v>Dell</v>
       </c>
       <c r="C24" t="str">
         <v>Dilshod</v>
       </c>
       <c r="D24">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F24">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25">
-        <v>24</v>
+      <c r="A25" t="str">
+        <v>5e57ee1bcf822f37ca4dd4c3</v>
       </c>
       <c r="B25" t="str">
-        <v>Mamur</v>
+        <v>Nozi</v>
       </c>
       <c r="C25" t="str">
-        <v>Dilshod</v>
+        <v>Oyatillo</v>
       </c>
       <c r="D25">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F25">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26">
-        <v>25</v>
-      </c>
-      <c r="B26" t="str">
-        <v>Sardor</v>
-      </c>
-      <c r="C26" t="str">
-        <v>Oyatillo</v>
-      </c>
-      <c r="D26">
-        <v>4</v>
-      </c>
-      <c r="F26">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27">
-        <v>26</v>
-      </c>
-      <c r="B27" t="str">
-        <v>Aziza</v>
-      </c>
-      <c r="C27" t="str">
-        <v>Dilshod</v>
-      </c>
-      <c r="D27">
-        <v>4</v>
-      </c>
-      <c r="F27">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28">
-        <v>27</v>
-      </c>
-      <c r="B28" t="str">
-        <v>Diyor</v>
-      </c>
-      <c r="C28" t="str">
-        <v>Dilshod</v>
-      </c>
-      <c r="D28">
-        <v>7</v>
-      </c>
-      <c r="F28">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29">
-        <v>28</v>
-      </c>
-      <c r="B29" t="str">
-        <v>Dell</v>
-      </c>
-      <c r="C29" t="str">
-        <v>Dilshod</v>
-      </c>
-      <c r="D29">
-        <v>6</v>
-      </c>
-      <c r="F29">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30">
-        <v>29</v>
-      </c>
-      <c r="B30" t="str">
-        <v>Nozi</v>
-      </c>
-      <c r="C30" t="str">
-        <v>Oyatillo</v>
-      </c>
-      <c r="D30">
-        <v>4</v>
-      </c>
-      <c r="F30">
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F30"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F25"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>